<commit_message>
Deleted note for non-respondent
</commit_message>
<xml_diff>
--- a/Assignments/A4/PhoneSurvey.xlsx
+++ b/Assignments/A4/PhoneSurvey.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="17">
   <si>
     <t>Survey Response sheet for MACS 30000 (Autumn 2018), Assignment 4</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t xml:space="preserve">jhn wolf, styart guarantee </t>
-  </si>
-  <si>
-    <t>Adam</t>
   </si>
   <si>
     <t>Invalid Number</t>
@@ -441,7 +438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,7 +449,7 @@
   <dimension ref="A1:BV204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+      <selection activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -485,7 +482,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:74">
@@ -501,7 +498,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:74">
@@ -517,7 +514,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:74">
@@ -533,7 +530,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:74">
@@ -549,7 +546,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:74">
@@ -565,7 +562,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:74">
@@ -581,7 +578,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:74">
@@ -597,7 +594,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:74">
@@ -613,7 +610,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:74" s="4" customFormat="1">
@@ -629,7 +626,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -797,7 +794,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:74">
@@ -813,7 +810,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:74">
@@ -829,7 +826,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:74">
@@ -845,7 +842,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:74">
@@ -861,7 +858,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:74">
@@ -877,7 +874,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:74">
@@ -893,7 +890,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:74">
@@ -909,7 +906,7 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:74">
@@ -925,7 +922,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:74">
@@ -941,7 +938,7 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:74" s="5" customFormat="1">
@@ -1053,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:74" s="4" customFormat="1">
@@ -1073,7 +1070,7 @@
         <v>48</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -1157,7 +1154,7 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:74">
@@ -1173,7 +1170,7 @@
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:74">
@@ -1189,7 +1186,7 @@
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:74">
@@ -1205,7 +1202,7 @@
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:74" s="4" customFormat="1">
@@ -1305,7 +1302,7 @@
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:74">
@@ -1321,7 +1318,7 @@
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:74" s="4" customFormat="1">
@@ -1589,7 +1586,7 @@
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:74" s="4" customFormat="1">
@@ -1689,7 +1686,7 @@
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:74" s="4" customFormat="1">
@@ -1709,7 +1706,7 @@
         <v>71</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
@@ -1793,7 +1790,7 @@
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:74">
@@ -1809,7 +1806,7 @@
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:74">
@@ -1825,7 +1822,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:74" s="4" customFormat="1">
@@ -1925,7 +1922,7 @@
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:74">
@@ -1941,7 +1938,7 @@
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:74">
@@ -1957,7 +1954,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:74">
@@ -1973,7 +1970,7 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:74">
@@ -1989,7 +1986,7 @@
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:74">
@@ -2005,7 +2002,7 @@
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:74">
@@ -2021,7 +2018,7 @@
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:74">
@@ -2037,7 +2034,7 @@
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:74">
@@ -2053,7 +2050,7 @@
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:74">
@@ -2069,7 +2066,7 @@
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:74" s="4" customFormat="1">
@@ -2169,7 +2166,7 @@
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:74">
@@ -2185,7 +2182,7 @@
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:74">
@@ -2201,7 +2198,7 @@
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:74" s="4" customFormat="1">
@@ -2301,7 +2298,7 @@
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:74">
@@ -2317,7 +2314,7 @@
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:74">
@@ -2333,7 +2330,7 @@
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:74">
@@ -2349,7 +2346,7 @@
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:74">
@@ -2365,7 +2362,7 @@
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:74">
@@ -2381,7 +2378,7 @@
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:74" s="4" customFormat="1">
@@ -2485,7 +2482,7 @@
         <v>50</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
@@ -2569,7 +2566,7 @@
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:74">
@@ -2585,7 +2582,7 @@
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:74" s="4" customFormat="1">
@@ -2685,7 +2682,7 @@
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:74">
@@ -2701,7 +2698,7 @@
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:74" ht="16.8" customHeight="1">
@@ -2717,7 +2714,7 @@
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:74" s="4" customFormat="1">
@@ -2901,7 +2898,7 @@
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:74">
@@ -2917,7 +2914,7 @@
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:74">
@@ -2933,7 +2930,7 @@
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:74">
@@ -2949,7 +2946,7 @@
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:74">
@@ -2965,7 +2962,7 @@
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
       <c r="F81" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:74">
@@ -2981,7 +2978,7 @@
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
       <c r="F82" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:74">
@@ -2997,7 +2994,7 @@
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:74" s="4" customFormat="1">
@@ -3097,7 +3094,7 @@
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="F85" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:74">
@@ -3113,7 +3110,7 @@
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:74" s="4" customFormat="1">
@@ -3297,7 +3294,7 @@
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:74">
@@ -3313,7 +3310,7 @@
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:74">
@@ -3329,7 +3326,7 @@
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
       <c r="F91" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:74">
@@ -3345,7 +3342,7 @@
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:74">
@@ -3361,7 +3358,7 @@
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
       <c r="F93" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:74" s="4" customFormat="1">
@@ -3461,7 +3458,7 @@
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
       <c r="F95" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:74">
@@ -3477,7 +3474,7 @@
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="F96" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:74">
@@ -3493,7 +3490,7 @@
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
       <c r="F97" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:74">
@@ -3509,7 +3506,7 @@
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
       <c r="F98" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:74">
@@ -3525,7 +3522,7 @@
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
       <c r="F99" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:74">
@@ -3541,7 +3538,7 @@
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
       <c r="F100" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:74">
@@ -3557,7 +3554,7 @@
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
       <c r="F101" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:74">
@@ -3573,7 +3570,7 @@
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
       <c r="F102" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:74">
@@ -3589,7 +3586,7 @@
       <c r="D103" s="5"/>
       <c r="E103" s="5"/>
       <c r="F103" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:74" s="4" customFormat="1">
@@ -3705,7 +3702,7 @@
       <c r="D106" s="5"/>
       <c r="E106" s="5"/>
       <c r="F106" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:74">
@@ -3721,7 +3718,7 @@
       <c r="D107" s="5"/>
       <c r="E107" s="5"/>
       <c r="F107" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:74">
@@ -3737,7 +3734,7 @@
       <c r="D108" s="5"/>
       <c r="E108" s="5"/>
       <c r="F108" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:74">
@@ -3769,7 +3766,7 @@
       <c r="D110" s="5"/>
       <c r="E110" s="5"/>
       <c r="F110" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:74">
@@ -3785,7 +3782,7 @@
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
       <c r="F111" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:74">
@@ -3819,7 +3816,7 @@
       <c r="D113" s="5"/>
       <c r="E113" s="5"/>
       <c r="F113" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:74">
@@ -3835,7 +3832,7 @@
       <c r="D114" s="5"/>
       <c r="E114" s="5"/>
       <c r="F114" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:74">
@@ -3851,7 +3848,7 @@
       <c r="D115" s="5"/>
       <c r="E115" s="5"/>
       <c r="F115" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:74">
@@ -3867,7 +3864,7 @@
       <c r="D116" s="5"/>
       <c r="E116" s="5"/>
       <c r="F116" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:74">
@@ -3883,7 +3880,7 @@
       <c r="D117" s="5"/>
       <c r="E117" s="5"/>
       <c r="F117" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:74">
@@ -3915,7 +3912,7 @@
       <c r="D119" s="5"/>
       <c r="E119" s="5"/>
       <c r="F119" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:74">
@@ -3931,7 +3928,7 @@
       <c r="D120" s="5"/>
       <c r="E120" s="5"/>
       <c r="F120" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:74">
@@ -3947,7 +3944,7 @@
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
       <c r="F121" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:74" s="4" customFormat="1">
@@ -4063,7 +4060,7 @@
       <c r="D124" s="5"/>
       <c r="E124" s="5"/>
       <c r="F124" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:74">
@@ -4079,7 +4076,7 @@
       <c r="D125" s="5"/>
       <c r="E125" s="5"/>
       <c r="F125" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:74">
@@ -4095,7 +4092,7 @@
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
       <c r="F126" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:74">
@@ -4111,7 +4108,7 @@
       <c r="D127" s="5"/>
       <c r="E127" s="5"/>
       <c r="F127" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:74">
@@ -4143,7 +4140,7 @@
       <c r="D129" s="5"/>
       <c r="E129" s="5"/>
       <c r="F129" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -4159,7 +4156,7 @@
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
       <c r="F130" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -4175,7 +4172,7 @@
       <c r="D131" s="5"/>
       <c r="E131" s="5"/>
       <c r="F131" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -4191,7 +4188,7 @@
       <c r="D132" s="5"/>
       <c r="E132" s="5"/>
       <c r="F132" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -4207,7 +4204,7 @@
       <c r="D133" s="5"/>
       <c r="E133" s="5"/>
       <c r="F133" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -4239,7 +4236,7 @@
       <c r="D135" s="5"/>
       <c r="E135" s="5"/>
       <c r="F135" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -4271,7 +4268,7 @@
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
       <c r="F137" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -4287,7 +4284,7 @@
       <c r="D138" s="5"/>
       <c r="E138" s="5"/>
       <c r="F138" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -4303,7 +4300,7 @@
       <c r="D139" s="5"/>
       <c r="E139" s="5"/>
       <c r="F139" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -4319,7 +4316,7 @@
       <c r="D140" s="5"/>
       <c r="E140" s="5"/>
       <c r="F140" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -4351,7 +4348,7 @@
       <c r="D142" s="5"/>
       <c r="E142" s="5"/>
       <c r="F142" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -4367,7 +4364,7 @@
       <c r="D143" s="5"/>
       <c r="E143" s="5"/>
       <c r="F143" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -4383,7 +4380,7 @@
       <c r="D144" s="5"/>
       <c r="E144" s="5"/>
       <c r="F144" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -4399,7 +4396,7 @@
       <c r="D145" s="5"/>
       <c r="E145" s="5"/>
       <c r="F145" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -4415,7 +4412,7 @@
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
       <c r="F146" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -4431,7 +4428,7 @@
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
       <c r="F147" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -4447,7 +4444,7 @@
       <c r="D148" s="5"/>
       <c r="E148" s="5"/>
       <c r="F148" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -4463,7 +4460,7 @@
       <c r="D149" s="5"/>
       <c r="E149" s="5"/>
       <c r="F149" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -4495,7 +4492,7 @@
       <c r="D151" s="5"/>
       <c r="E151" s="5"/>
       <c r="F151" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -4543,7 +4540,7 @@
       <c r="D154" s="5"/>
       <c r="E154" s="5"/>
       <c r="F154" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -4559,7 +4556,7 @@
       <c r="D155" s="5"/>
       <c r="E155" s="5"/>
       <c r="F155" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -4591,7 +4588,7 @@
       <c r="D157" s="5"/>
       <c r="E157" s="5"/>
       <c r="F157" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -4607,7 +4604,7 @@
       <c r="D158" s="5"/>
       <c r="E158" s="5"/>
       <c r="F158" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -4623,7 +4620,7 @@
       <c r="D159" s="5"/>
       <c r="E159" s="5"/>
       <c r="F159" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -4655,7 +4652,7 @@
       <c r="D161" s="5"/>
       <c r="E161" s="5"/>
       <c r="F161" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -4671,7 +4668,7 @@
       <c r="D162" s="5"/>
       <c r="E162" s="5"/>
       <c r="F162" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -4687,7 +4684,7 @@
       <c r="D163" s="5"/>
       <c r="E163" s="5"/>
       <c r="F163" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -4703,7 +4700,7 @@
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
       <c r="F164" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:6">
@@ -4719,7 +4716,7 @@
       <c r="D165" s="5"/>
       <c r="E165" s="5"/>
       <c r="F165" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -4733,9 +4730,7 @@
         <v>0</v>
       </c>
       <c r="D166" s="5"/>
-      <c r="E166" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="E166" s="5"/>
       <c r="F166" s="5" t="s">
         <v>7</v>
       </c>
@@ -4769,7 +4764,7 @@
       <c r="D168" s="5"/>
       <c r="E168" s="5"/>
       <c r="F168" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -4785,7 +4780,7 @@
       <c r="D169" s="5"/>
       <c r="E169" s="5"/>
       <c r="F169" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -4801,7 +4796,7 @@
       <c r="D170" s="5"/>
       <c r="E170" s="5"/>
       <c r="F170" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -4817,7 +4812,7 @@
       <c r="D171" s="5"/>
       <c r="E171" s="5"/>
       <c r="F171" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -4833,7 +4828,7 @@
       <c r="D172" s="5"/>
       <c r="E172" s="5"/>
       <c r="F172" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -4849,7 +4844,7 @@
       <c r="D173" s="5"/>
       <c r="E173" s="5"/>
       <c r="F173" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -4865,7 +4860,7 @@
       <c r="D174" s="5"/>
       <c r="E174" s="5"/>
       <c r="F174" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:6">
@@ -4881,7 +4876,7 @@
       <c r="D175" s="5"/>
       <c r="E175" s="5"/>
       <c r="F175" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -4913,7 +4908,7 @@
       <c r="D177" s="5"/>
       <c r="E177" s="5"/>
       <c r="F177" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -4929,7 +4924,7 @@
       <c r="D178" s="5"/>
       <c r="E178" s="5"/>
       <c r="F178" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -4945,7 +4940,7 @@
       <c r="D179" s="5"/>
       <c r="E179" s="5"/>
       <c r="F179" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -4961,7 +4956,7 @@
       <c r="D180" s="5"/>
       <c r="E180" s="5"/>
       <c r="F180" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -4977,7 +4972,7 @@
       <c r="D181" s="5"/>
       <c r="E181" s="5"/>
       <c r="F181" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -4993,7 +4988,7 @@
       <c r="D182" s="5"/>
       <c r="E182" s="5"/>
       <c r="F182" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -5025,7 +5020,7 @@
       <c r="D184" s="5"/>
       <c r="E184" s="5"/>
       <c r="F184" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:6">
@@ -5057,7 +5052,7 @@
       <c r="D186" s="5"/>
       <c r="E186" s="5"/>
       <c r="F186" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -5073,7 +5068,7 @@
       <c r="D187" s="5"/>
       <c r="E187" s="5"/>
       <c r="F187" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -5105,7 +5100,7 @@
       <c r="D189" s="5"/>
       <c r="E189" s="5"/>
       <c r="F189" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -5121,7 +5116,7 @@
       <c r="D190" s="5"/>
       <c r="E190" s="5"/>
       <c r="F190" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -5137,7 +5132,7 @@
       <c r="D191" s="5"/>
       <c r="E191" s="5"/>
       <c r="F191" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -5169,7 +5164,7 @@
       <c r="D193" s="5"/>
       <c r="E193" s="5"/>
       <c r="F193" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -5185,7 +5180,7 @@
       <c r="D194" s="5"/>
       <c r="E194" s="5"/>
       <c r="F194" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:6">
@@ -5201,7 +5196,7 @@
       <c r="D195" s="5"/>
       <c r="E195" s="5"/>
       <c r="F195" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:6">
@@ -5217,7 +5212,7 @@
       <c r="D196" s="5"/>
       <c r="E196" s="5"/>
       <c r="F196" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:6">
@@ -5233,7 +5228,7 @@
       <c r="D197" s="5"/>
       <c r="E197" s="5"/>
       <c r="F197" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -5249,7 +5244,7 @@
       <c r="D198" s="5"/>
       <c r="E198" s="5"/>
       <c r="F198" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:6">
@@ -5265,7 +5260,7 @@
       <c r="D199" s="5"/>
       <c r="E199" s="5"/>
       <c r="F199" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:6">
@@ -5297,7 +5292,7 @@
       <c r="D201" s="5"/>
       <c r="E201" s="5"/>
       <c r="F201" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -5313,7 +5308,7 @@
       <c r="D202" s="5"/>
       <c r="E202" s="5"/>
       <c r="F202" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:6">
@@ -5329,7 +5324,7 @@
       <c r="D203" s="5"/>
       <c r="E203" s="5"/>
       <c r="F203" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:6">

</xml_diff>